<commit_message>
Poprawne działanie rejestrowania, dodanie hasła(bo zapomniałem),
</commit_message>
<xml_diff>
--- a/database/drugs.xlsx
+++ b/database/drugs.xlsx
@@ -468,7 +468,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
@@ -500,7 +500,7 @@
         <v>22</v>
       </c>
       <c r="D4" t="n">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>